<commit_message>
More accurate directional calculations
</commit_message>
<xml_diff>
--- a/tests/group.xlsx
+++ b/tests/group.xlsx
@@ -343,7 +343,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -354,7 +354,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -508,7 +508,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>